<commit_message>
Remove names from new data
</commit_message>
<xml_diff>
--- a/data/correlation_analysis_timeout_max.xlsx
+++ b/data/correlation_analysis_timeout_max.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0E82EC7-9666-4A45-BA40-2DD75BC0DA9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_tools" sheetId="1" r:id="rId1"/>
@@ -13,7 +14,7 @@
     <sheet name="infer" sheetId="4" r:id="rId4"/>
     <sheet name="openjml" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -140,8 +141,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,6 +205,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -250,7 +259,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -282,9 +291,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -316,6 +343,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -491,12 +536,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.7109375" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
@@ -508,11 +553,10 @@
     <col min="8" max="8" width="28.7109375" customWidth="1"/>
     <col min="9" max="9" width="21.7109375" customWidth="1"/>
     <col min="10" max="10" width="20.7109375" customWidth="1"/>
-    <col min="11" max="11" width="21.7109375" customWidth="1"/>
-    <col min="12" max="12" width="21.7109375" customWidth="1"/>
+    <col min="11" max="12" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -550,7 +594,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -576,19 +620,19 @@
         <v>23</v>
       </c>
       <c r="I2">
-        <v>-0.3377277477430254</v>
+        <v>-0.33772774774302539</v>
       </c>
       <c r="J2">
-        <v>0.03761941401427579</v>
+        <v>3.7619414014275793E-2</v>
       </c>
       <c r="K2">
-        <v>-0.3976802252851466</v>
+        <v>-0.39768022528514663</v>
       </c>
       <c r="L2">
-        <v>0.06021635626528627</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+        <v>6.0216356265286271E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -614,19 +658,19 @@
         <v>23</v>
       </c>
       <c r="I3">
-        <v>-0.4275482906928738</v>
+        <v>-0.42754829069287381</v>
       </c>
       <c r="J3">
-        <v>0.007641040482277836</v>
+        <v>7.6410404822778357E-3</v>
       </c>
       <c r="K3">
-        <v>-0.5452867412432369</v>
+        <v>-0.54528674124323695</v>
       </c>
       <c r="L3">
-        <v>0.007124393687845218</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+        <v>7.124393687845218E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -652,19 +696,19 @@
         <v>23</v>
       </c>
       <c r="I4">
-        <v>0.4111706600105638</v>
+        <v>0.41117066001056379</v>
       </c>
       <c r="J4">
-        <v>0.00982101261512518</v>
+        <v>9.8210126151251805E-3</v>
       </c>
       <c r="K4">
-        <v>0.5360003171861121</v>
+        <v>0.53600031718611207</v>
       </c>
       <c r="L4">
-        <v>0.008382091244079634</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
+        <v>8.3820912440796345E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -690,19 +734,19 @@
         <v>12</v>
       </c>
       <c r="I5">
-        <v>-0.3133397807202561</v>
+        <v>-0.31333978072025609</v>
       </c>
       <c r="J5">
-        <v>0.1884699909010059</v>
+        <v>0.18846999090100591</v>
       </c>
       <c r="K5">
-        <v>-0.3178304128441319</v>
+        <v>-0.31783041284413188</v>
       </c>
       <c r="L5">
-        <v>0.3140610795011266</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
+        <v>0.31406107950112661</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -728,19 +772,19 @@
         <v>12</v>
       </c>
       <c r="I6">
-        <v>-0.4526019054848143</v>
+        <v>-0.45260190548481433</v>
       </c>
       <c r="J6">
-        <v>0.05748353173133636</v>
+        <v>5.7483531731336357E-2</v>
       </c>
       <c r="K6">
-        <v>-0.4693542143163343</v>
+        <v>-0.46935421431633428</v>
       </c>
       <c r="L6">
-        <v>0.1237049815910057</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
+        <v>0.12370498159100569</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -766,19 +810,19 @@
         <v>12</v>
       </c>
       <c r="I7">
-        <v>-0.3829708431025352</v>
+        <v>-0.38297084310253521</v>
       </c>
       <c r="J7">
         <v>0.1079738014574666</v>
       </c>
       <c r="K7">
-        <v>-0.458267106891539</v>
+        <v>-0.45826710689153899</v>
       </c>
       <c r="L7">
-        <v>0.1340598783554668</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
+        <v>0.13405987835546679</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -804,19 +848,19 @@
         <v>12</v>
       </c>
       <c r="I8">
-        <v>0.1392621247645583</v>
+        <v>0.13926212476455829</v>
       </c>
       <c r="J8">
         <v>0.5588858290416201</v>
       </c>
       <c r="K8">
-        <v>0.2032636361212471</v>
+        <v>0.20326363612124709</v>
       </c>
       <c r="L8">
-        <v>0.5263323724525723</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+        <v>0.52633237245257225</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -842,19 +886,19 @@
         <v>100</v>
       </c>
       <c r="I9">
-        <v>-0.1679930849817192</v>
+        <v>-0.16799308498171919</v>
       </c>
       <c r="J9">
-        <v>0.01571209940531982</v>
+        <v>1.571209940531982E-2</v>
       </c>
       <c r="K9">
-        <v>-0.2581562594294852</v>
+        <v>-0.25815625942948522</v>
       </c>
       <c r="L9">
-        <v>0.009508181415596517</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
+        <v>9.5081814155965165E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -880,19 +924,19 @@
         <v>50</v>
       </c>
       <c r="I10">
-        <v>-0.01788960397609135</v>
+        <v>-1.7889603976091351E-2</v>
       </c>
       <c r="J10">
-        <v>0.8831700141519032</v>
+        <v>0.88317001415190322</v>
       </c>
       <c r="K10">
-        <v>-0.01605248793883186</v>
+        <v>-1.605248793883186E-2</v>
       </c>
       <c r="L10">
-        <v>0.9118983828429555</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
+        <v>0.91189838284295555</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -918,19 +962,19 @@
         <v>50</v>
       </c>
       <c r="I11">
-        <v>-0.0319066731228802</v>
+        <v>-3.1906673122880203E-2</v>
       </c>
       <c r="J11">
-        <v>0.7837672300250216</v>
+        <v>0.78376723002502158</v>
       </c>
       <c r="K11">
-        <v>-0.03045075791865187</v>
+        <v>-3.0450757918651868E-2</v>
       </c>
       <c r="L11">
-        <v>0.8337285990222609</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
+        <v>0.83372859902226093</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -959,16 +1003,16 @@
         <v>-0.2441570787714312</v>
       </c>
       <c r="J12">
-        <v>0.03455416553919029</v>
+        <v>3.4554165539190287E-2</v>
       </c>
       <c r="K12">
         <v>-0.3094340106343606</v>
       </c>
       <c r="L12">
-        <v>0.02876701130235894</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
+        <v>2.8767011302358939E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -994,19 +1038,19 @@
         <v>10</v>
       </c>
       <c r="I13">
-        <v>-0.4535394202249742</v>
+        <v>-0.45353942022497418</v>
       </c>
       <c r="J13">
-        <v>0.08070214265077501</v>
+        <v>8.0702142650775008E-2</v>
       </c>
       <c r="K13">
-        <v>-0.5512130501182249</v>
+        <v>-0.55121305011822486</v>
       </c>
       <c r="L13">
-        <v>0.09862398123473154</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
+        <v>9.8623981234731539E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -1032,19 +1076,19 @@
         <v>10</v>
       </c>
       <c r="I14">
-        <v>-0.02387049580131443</v>
+        <v>-2.387049580131443E-2</v>
       </c>
       <c r="J14">
-        <v>0.92675547372309</v>
+        <v>0.92675547372308997</v>
       </c>
       <c r="K14">
-        <v>-0.09290107586262218</v>
+        <v>-9.2901075862622182E-2</v>
       </c>
       <c r="L14">
-        <v>0.7985237548304135</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
+        <v>0.79852375483041349</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -1070,19 +1114,19 @@
         <v>10</v>
       </c>
       <c r="I15">
-        <v>0.09656090991705352</v>
+        <v>9.6560909917053517E-2</v>
       </c>
       <c r="J15">
-        <v>0.7120793980044939</v>
+        <v>0.71207939800449394</v>
       </c>
       <c r="K15">
-        <v>0.1428819499477476</v>
+        <v>0.14288194994774761</v>
       </c>
       <c r="L15">
-        <v>0.6937488280957302</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
+        <v>0.69374882809573024</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -1108,19 +1152,19 @@
         <v>10</v>
       </c>
       <c r="I16">
-        <v>-0.7399853698407473</v>
+        <v>-0.73998536984074725</v>
       </c>
       <c r="J16">
-        <v>0.004375235749920733</v>
+        <v>4.375235749920733E-3</v>
       </c>
       <c r="K16">
-        <v>-0.8670767080511405</v>
+        <v>-0.86707670805114045</v>
       </c>
       <c r="L16">
-        <v>0.001159768265192443</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
+        <v>1.1597682651924429E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -1146,19 +1190,19 @@
         <v>10</v>
       </c>
       <c r="I17">
-        <v>-0.3103164454170876</v>
+        <v>-0.31031644541708758</v>
       </c>
       <c r="J17">
         <v>0.2320634889020341</v>
       </c>
       <c r="K17">
-        <v>-0.4149581388530457</v>
+        <v>-0.41495813885304572</v>
       </c>
       <c r="L17">
         <v>0.233093730241445</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -1184,19 +1228,19 @@
         <v>10</v>
       </c>
       <c r="I18">
-        <v>0.4535394202249742</v>
+        <v>0.45353942022497418</v>
       </c>
       <c r="J18">
-        <v>0.08070214265077501</v>
+        <v>8.0702142650775008E-2</v>
       </c>
       <c r="K18">
-        <v>0.5635998602332413</v>
+        <v>0.56359986023324127</v>
       </c>
       <c r="L18">
-        <v>0.08974939558201678</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
+        <v>8.9749395582016778E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -1222,19 +1266,19 @@
         <v>10</v>
       </c>
       <c r="I19">
-        <v>0.4828045495852675</v>
+        <v>0.48280454958526747</v>
       </c>
       <c r="J19">
-        <v>0.06499039472076076</v>
+        <v>6.4990394720760764E-2</v>
       </c>
       <c r="K19">
-        <v>0.5932707052178214</v>
+        <v>0.59327070521782144</v>
       </c>
       <c r="L19">
-        <v>0.0706202179291523</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12">
+        <v>7.0620217929152296E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -1260,19 +1304,19 @@
         <v>10</v>
       </c>
       <c r="I20">
-        <v>-0.3580574370197164</v>
+        <v>-0.35805743701971637</v>
       </c>
       <c r="J20">
-        <v>0.1679207532945924</v>
+        <v>0.16792075329459241</v>
       </c>
       <c r="K20">
-        <v>-0.4954724046006516</v>
+        <v>-0.49547240460065162</v>
       </c>
       <c r="L20">
-        <v>0.1453294522910624</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12">
+        <v>0.14532945229106239</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -1298,19 +1342,19 @@
         <v>10</v>
       </c>
       <c r="I21">
-        <v>-0.4535394202249742</v>
+        <v>-0.45353942022497418</v>
       </c>
       <c r="J21">
-        <v>0.08070214265077501</v>
+        <v>8.0702142650775008E-2</v>
       </c>
       <c r="K21">
-        <v>-0.6007602905782901</v>
+        <v>-0.60076029057829006</v>
       </c>
       <c r="L21">
-        <v>0.06625295074379814</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12">
+        <v>6.6252950743798139E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -1339,16 +1383,16 @@
         <v>0.1193524790065721</v>
       </c>
       <c r="J22">
-        <v>0.6457756768370824</v>
+        <v>0.64577567683708237</v>
       </c>
       <c r="K22">
-        <v>0.1486417213801955</v>
+        <v>0.14864172138019549</v>
       </c>
       <c r="L22">
-        <v>0.6819355638686473</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12">
+        <v>0.68193556386864729</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -1374,19 +1418,19 @@
         <v>10</v>
       </c>
       <c r="I23">
-        <v>0.167093470609201</v>
+        <v>0.16709347060920099</v>
       </c>
       <c r="J23">
-        <v>0.5199036173455835</v>
+        <v>0.51990361734558355</v>
       </c>
       <c r="K23">
-        <v>0.2725098225303584</v>
+        <v>0.27250982253035838</v>
       </c>
       <c r="L23">
-        <v>0.446215643690079</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12">
+        <v>0.44621564369007899</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -1412,19 +1456,19 @@
         <v>10</v>
       </c>
       <c r="I24">
-        <v>-0.3580574370197164</v>
+        <v>-0.35805743701971637</v>
       </c>
       <c r="J24">
-        <v>0.1679207532945924</v>
+        <v>0.16792075329459241</v>
       </c>
       <c r="K24">
-        <v>-0.4706987843706191</v>
+        <v>-0.47069878437061913</v>
       </c>
       <c r="L24">
         <v>0.1697475039817557</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -1450,19 +1494,19 @@
         <v>16</v>
       </c>
       <c r="I25">
-        <v>-0.1807753815155468</v>
+        <v>-0.18077538151554681</v>
       </c>
       <c r="J25">
-        <v>0.3541954904764164</v>
+        <v>0.35419549047641641</v>
       </c>
       <c r="K25">
-        <v>-0.2576049186596542</v>
+        <v>-0.25760491865965418</v>
       </c>
       <c r="L25">
-        <v>0.3354345184285685</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12">
+        <v>0.33543451842856847</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -1488,19 +1532,19 @@
         <v>16</v>
       </c>
       <c r="I26">
-        <v>-0.1807753815155468</v>
+        <v>-0.18077538151554681</v>
       </c>
       <c r="J26">
-        <v>0.3541954904764164</v>
+        <v>0.35419549047641641</v>
       </c>
       <c r="K26">
-        <v>-0.2666436877354316</v>
+        <v>-0.26664368773543162</v>
       </c>
       <c r="L26">
-        <v>0.3181414648703181</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12">
+        <v>0.31814146487031808</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -1526,19 +1570,19 @@
         <v>16</v>
       </c>
       <c r="I27">
-        <v>0.3539900381483285</v>
+        <v>0.35399003814832852</v>
       </c>
       <c r="J27">
-        <v>0.07056136851892029</v>
+        <v>7.0561368518920295E-2</v>
       </c>
       <c r="K27">
-        <v>0.4341802833034056</v>
+        <v>0.43418028330340558</v>
       </c>
       <c r="L27">
-        <v>0.09288178063084394</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12">
+        <v>9.2881780630843944E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -1567,16 +1611,16 @@
         <v>-0.1647705109143269</v>
       </c>
       <c r="J28">
-        <v>0.4027546538976249</v>
+        <v>0.40275465389762488</v>
       </c>
       <c r="K28">
         <v>-0.2493004677260264</v>
       </c>
       <c r="L28">
-        <v>0.3517858440384553</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12">
+        <v>0.35178584403845531</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>18</v>
       </c>
@@ -1605,27 +1649,28 @@
         <v>-0.1265427670608828</v>
       </c>
       <c r="J29">
-        <v>0.5166373798159882</v>
+        <v>0.51663737981598823</v>
       </c>
       <c r="K29">
         <v>-0.1491396897503261</v>
       </c>
       <c r="L29">
-        <v>0.5814513259975999</v>
+        <v>0.58145132599759985</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.7109375" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
@@ -1636,12 +1681,11 @@
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
     <col min="8" max="8" width="28.7109375" customWidth="1"/>
     <col min="9" max="9" width="21.7109375" customWidth="1"/>
-    <col min="10" max="10" width="20.7109375" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+    <col min="10" max="11" width="20.7109375" customWidth="1"/>
     <col min="12" max="12" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1679,7 +1723,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1708,16 +1752,16 @@
         <v>-0.2277100170213244</v>
       </c>
       <c r="J2">
-        <v>0.2003280221869526</v>
+        <v>0.20032802218695259</v>
       </c>
       <c r="K2">
-        <v>-0.2719723502938716</v>
+        <v>-0.27197235029387162</v>
       </c>
       <c r="L2">
-        <v>0.2093250956596323</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+        <v>0.20932509565963231</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1743,19 +1787,19 @@
         <v>23</v>
       </c>
       <c r="I3">
-        <v>-0.263477777620917</v>
+        <v>-0.26347777762091701</v>
       </c>
       <c r="J3">
         <v>0.1329850671160174</v>
       </c>
       <c r="K3">
-        <v>-0.3201778730528596</v>
+        <v>-0.32017787305285961</v>
       </c>
       <c r="L3">
-        <v>0.1363764100850406</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+        <v>0.13637641008504059</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1784,16 +1828,16 @@
         <v>0.2297034206521828</v>
       </c>
       <c r="J4">
-        <v>0.187290841633909</v>
+        <v>0.18729084163390899</v>
       </c>
       <c r="K4">
-        <v>0.2809695424230301</v>
+        <v>0.28096954242303013</v>
       </c>
       <c r="L4">
-        <v>0.1940516726155841</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
+        <v>0.19405167261558409</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1819,7 +1863,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1845,7 +1889,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1871,7 +1915,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1897,7 +1941,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1923,19 +1967,19 @@
         <v>100</v>
       </c>
       <c r="I9">
-        <v>-0.2289041597670328</v>
+        <v>-0.22890415976703279</v>
       </c>
       <c r="J9">
-        <v>0.004154062204876697</v>
+        <v>4.1540622048766972E-3</v>
       </c>
       <c r="K9">
-        <v>-0.2872671746617843</v>
+        <v>-0.28726717466178431</v>
       </c>
       <c r="L9">
-        <v>0.003756720549751365</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
+        <v>3.7567205497513649E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1961,19 +2005,19 @@
         <v>50</v>
       </c>
       <c r="I10">
-        <v>-0.01788960397609135</v>
+        <v>-1.7889603976091351E-2</v>
       </c>
       <c r="J10">
-        <v>0.8831700141519032</v>
+        <v>0.88317001415190322</v>
       </c>
       <c r="K10">
-        <v>-0.02174552145202223</v>
+        <v>-2.1745521452022229E-2</v>
       </c>
       <c r="L10">
-        <v>0.8808493755591094</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
+        <v>0.88084937555910936</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1999,19 +2043,19 @@
         <v>50</v>
       </c>
       <c r="I11">
-        <v>-0.02439922062337898</v>
+        <v>-2.439922062337898E-2</v>
       </c>
       <c r="J11">
-        <v>0.8337884478927275</v>
+        <v>0.83378844789272755</v>
       </c>
       <c r="K11">
-        <v>-0.02805160729475809</v>
+        <v>-2.8051607294758089E-2</v>
       </c>
       <c r="L11">
-        <v>0.8466646412386398</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
+        <v>0.84666464123863983</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -2037,19 +2081,19 @@
         <v>50</v>
       </c>
       <c r="I12">
-        <v>-0.2516122567491849</v>
+        <v>-0.25161225674918491</v>
       </c>
       <c r="J12">
-        <v>0.02940004335865699</v>
+        <v>2.940004335865699E-2</v>
       </c>
       <c r="K12">
-        <v>-0.3118320089283974</v>
+        <v>-0.31183200892839741</v>
       </c>
       <c r="L12">
-        <v>0.02748882596687927</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
+        <v>2.7488825966879269E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -2075,19 +2119,19 @@
         <v>10</v>
       </c>
       <c r="I13">
-        <v>0.3651483716701108</v>
+        <v>0.36514837167011083</v>
       </c>
       <c r="J13">
-        <v>0.2008251226951454</v>
+        <v>0.20082512269514541</v>
       </c>
       <c r="K13">
-        <v>0.4264014327112208</v>
+        <v>0.42640143271122077</v>
       </c>
       <c r="L13">
-        <v>0.2191383605228726</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
+        <v>0.21913836052287261</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -2113,19 +2157,19 @@
         <v>10</v>
       </c>
       <c r="I14">
-        <v>0.7302967433402215</v>
+        <v>0.73029674334022154</v>
       </c>
       <c r="J14">
-        <v>0.01051524593585891</v>
+        <v>1.0515245935858911E-2</v>
       </c>
       <c r="K14">
-        <v>0.8528028654224417</v>
+        <v>0.85280286542244166</v>
       </c>
       <c r="L14">
-        <v>0.001712874149321468</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
+        <v>1.712874149321468E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -2151,19 +2195,19 @@
         <v>10</v>
       </c>
       <c r="I15">
-        <v>0.7385489458759965</v>
+        <v>0.73854894587599651</v>
       </c>
       <c r="J15">
-        <v>0.01028204822194895</v>
+        <v>1.0282048221948951E-2</v>
       </c>
       <c r="K15">
-        <v>0.8553989227683017</v>
+        <v>0.85539892276830165</v>
       </c>
       <c r="L15">
-        <v>0.001600453316805279</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
+        <v>1.600453316805279E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -2192,16 +2236,16 @@
         <v>-0.1217161238900369</v>
       </c>
       <c r="J16">
-        <v>0.6698153575994166</v>
+        <v>0.66981535759941657</v>
       </c>
       <c r="K16">
         <v>-0.1421338109037403</v>
       </c>
       <c r="L16">
-        <v>0.6952876854012655</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
+        <v>0.69528768540126551</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -2227,19 +2271,19 @@
         <v>10</v>
       </c>
       <c r="I17">
-        <v>-0.5477225575051662</v>
+        <v>-0.54772255750516619</v>
       </c>
       <c r="J17">
-        <v>0.05500883362926572</v>
+        <v>5.5008833629265723E-2</v>
       </c>
       <c r="K17">
-        <v>-0.6396021490668313</v>
+        <v>-0.63960214906683133</v>
       </c>
       <c r="L17">
-        <v>0.04643461767158175</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
+        <v>4.6434617671581753E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -2265,19 +2309,19 @@
         <v>10</v>
       </c>
       <c r="I18">
-        <v>-0.3651483716701108</v>
+        <v>-0.36514837167011083</v>
       </c>
       <c r="J18">
-        <v>0.2008251226951454</v>
+        <v>0.20082512269514541</v>
       </c>
       <c r="K18">
-        <v>-0.4264014327112208</v>
+        <v>-0.42640143271122077</v>
       </c>
       <c r="L18">
-        <v>0.2191383605228726</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
+        <v>0.21913836052287261</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -2303,19 +2347,19 @@
         <v>10</v>
       </c>
       <c r="I19">
-        <v>-0.3077287274483319</v>
+        <v>-0.30772872744833191</v>
       </c>
       <c r="J19">
-        <v>0.2849576406684299</v>
+        <v>0.28495764066842988</v>
       </c>
       <c r="K19">
-        <v>-0.3564162178201257</v>
+        <v>-0.35641621782012572</v>
       </c>
       <c r="L19">
-        <v>0.312061132326838</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12">
+        <v>0.31206113232683802</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -2344,16 +2388,16 @@
         <v>0.3042903097250923</v>
       </c>
       <c r="J20">
-        <v>0.2864220227778588</v>
+        <v>0.28642202277785878</v>
       </c>
       <c r="K20">
-        <v>0.3553345272593507</v>
+        <v>0.35533452725935072</v>
       </c>
       <c r="L20">
-        <v>0.3136373640754537</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12">
+        <v>0.31363736407545367</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -2379,19 +2423,19 @@
         <v>10</v>
       </c>
       <c r="I21">
-        <v>-0.3651483716701108</v>
+        <v>-0.36514837167011083</v>
       </c>
       <c r="J21">
-        <v>0.2008251226951454</v>
+        <v>0.20082512269514541</v>
       </c>
       <c r="K21">
-        <v>-0.4264014327112208</v>
+        <v>-0.42640143271122077</v>
       </c>
       <c r="L21">
-        <v>0.2191383605228726</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12">
+        <v>0.21913836052287261</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -2420,16 +2464,16 @@
         <v>0.3042903097250923</v>
       </c>
       <c r="J22">
-        <v>0.2864220227778588</v>
+        <v>0.28642202277785878</v>
       </c>
       <c r="K22">
-        <v>0.3553345272593507</v>
+        <v>0.35533452725935072</v>
       </c>
       <c r="L22">
-        <v>0.3136373640754537</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12">
+        <v>0.31363736407545367</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -2455,19 +2499,19 @@
         <v>10</v>
       </c>
       <c r="I23">
-        <v>0.3651483716701108</v>
+        <v>0.36514837167011083</v>
       </c>
       <c r="J23">
-        <v>0.2008251226951454</v>
+        <v>0.20082512269514541</v>
       </c>
       <c r="K23">
-        <v>0.4264014327112208</v>
+        <v>0.42640143271122077</v>
       </c>
       <c r="L23">
-        <v>0.2191383605228726</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12">
+        <v>0.21913836052287261</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -2493,19 +2537,19 @@
         <v>10</v>
       </c>
       <c r="I24">
-        <v>-0.4260064336151292</v>
+        <v>-0.42600643361512919</v>
       </c>
       <c r="J24">
-        <v>0.1355930012663022</v>
+        <v>0.13559300126630219</v>
       </c>
       <c r="K24">
         <v>-0.497468338163091</v>
       </c>
       <c r="L24">
-        <v>0.1434614655950857</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12">
+        <v>0.14346146559508571</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -2531,19 +2575,19 @@
         <v>16</v>
       </c>
       <c r="I25">
-        <v>-0.1023234355858201</v>
+        <v>-0.10232343558582011</v>
       </c>
       <c r="J25">
-        <v>0.6377328900501884</v>
+        <v>0.63773289005018841</v>
       </c>
       <c r="K25">
-        <v>-0.1215783580010781</v>
+        <v>-0.12157835800107809</v>
       </c>
       <c r="L25">
-        <v>0.6537671093538482</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12">
+        <v>0.65376710935384819</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -2569,19 +2613,19 @@
         <v>16</v>
       </c>
       <c r="I26">
-        <v>-0.01461763365511715</v>
+        <v>-1.4617633655117149E-2</v>
       </c>
       <c r="J26">
-        <v>0.94636892512424</v>
+        <v>0.94636892512423998</v>
       </c>
       <c r="K26">
-        <v>-0.01736833685729687</v>
+        <v>-1.736833685729687E-2</v>
       </c>
       <c r="L26">
-        <v>0.949096032737041</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12">
+        <v>0.94909603273704102</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -2607,19 +2651,19 @@
         <v>16</v>
       </c>
       <c r="I27">
-        <v>0.2788995520575487</v>
+        <v>0.27889955205754868</v>
       </c>
       <c r="J27">
-        <v>0.2008903265397131</v>
+        <v>0.20089032653971309</v>
       </c>
       <c r="K27">
         <v>0.3302413141237342</v>
       </c>
       <c r="L27">
-        <v>0.2115824618683086</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12">
+        <v>0.21158246186830859</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -2645,19 +2689,19 @@
         <v>16</v>
       </c>
       <c r="I28">
-        <v>-0.1628423836175867</v>
+        <v>-0.16284238361758671</v>
       </c>
       <c r="J28">
-        <v>0.458010988385219</v>
+        <v>0.45801098838521898</v>
       </c>
       <c r="K28">
-        <v>-0.1916161134706239</v>
+        <v>-0.19161611347062391</v>
       </c>
       <c r="L28">
         <v>0.4771333722542902</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>18</v>
       </c>
@@ -2683,30 +2727,31 @@
         <v>16</v>
       </c>
       <c r="I29">
-        <v>-0.2484997721369916</v>
+        <v>-0.24849977213699159</v>
       </c>
       <c r="J29">
-        <v>0.2528129010164081</v>
+        <v>0.25281290101640808</v>
       </c>
       <c r="K29">
-        <v>-0.2952617265740468</v>
+        <v>-0.29526172657404681</v>
       </c>
       <c r="L29">
-        <v>0.2669012522950682</v>
+        <v>0.26690125229506823</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.7109375" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
@@ -2722,7 +2767,7 @@
     <col min="12" max="12" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2760,7 +2805,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2786,19 +2831,19 @@
         <v>23</v>
       </c>
       <c r="I2">
-        <v>-0.1707825127659933</v>
+        <v>-0.17078251276599329</v>
       </c>
       <c r="J2">
         <v>0.3368221511559395</v>
       </c>
       <c r="K2">
-        <v>-0.2206327958702234</v>
+        <v>-0.22063279587022341</v>
       </c>
       <c r="L2">
-        <v>0.3117066831945562</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+        <v>0.31170668319455619</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -2824,19 +2869,19 @@
         <v>23</v>
       </c>
       <c r="I3">
-        <v>-0.2155727271443866</v>
+        <v>-0.21557272714438661</v>
       </c>
       <c r="J3">
         <v>0.2189727791934982</v>
       </c>
       <c r="K3">
-        <v>-0.2830068271047704</v>
+        <v>-0.28300682710477038</v>
       </c>
       <c r="L3">
-        <v>0.1907013837125806</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+        <v>0.19070138371258061</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -2865,16 +2910,16 @@
         <v>0.182178575000007</v>
       </c>
       <c r="J4">
-        <v>0.2956465760209075</v>
+        <v>0.29564657602090749</v>
       </c>
       <c r="K4">
-        <v>0.2404694281998906</v>
+        <v>0.24046942819989059</v>
       </c>
       <c r="L4">
-        <v>0.2690489763203219</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
+        <v>0.26904897632032188</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -2900,19 +2945,19 @@
         <v>12</v>
       </c>
       <c r="I5">
-        <v>-0.1113404428537808</v>
+        <v>-0.11134044285378079</v>
       </c>
       <c r="J5">
-        <v>0.6639079018776488</v>
+        <v>0.66390790187764881</v>
       </c>
       <c r="K5">
-        <v>-0.131013944022344</v>
+        <v>-0.13101394402234401</v>
       </c>
       <c r="L5">
-        <v>0.6848487144273757</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
+        <v>0.68484871442737572</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -2938,19 +2983,19 @@
         <v>12</v>
       </c>
       <c r="I6">
-        <v>-0.2597943666588219</v>
+        <v>-0.25979436665882188</v>
       </c>
       <c r="J6">
-        <v>0.3106354563374008</v>
+        <v>0.31063545633740081</v>
       </c>
       <c r="K6">
-        <v>-0.3056992027188027</v>
+        <v>-0.30569920271880269</v>
       </c>
       <c r="L6">
-        <v>0.3338931364506602</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
+        <v>0.33389313645066021</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -2976,19 +3021,19 @@
         <v>12</v>
       </c>
       <c r="I7">
-        <v>0.1113404428537808</v>
+        <v>0.11134044285378079</v>
       </c>
       <c r="J7">
-        <v>0.6639079018776488</v>
+        <v>0.66390790187764881</v>
       </c>
       <c r="K7">
-        <v>0.131013944022344</v>
+        <v>0.13101394402234401</v>
       </c>
       <c r="L7">
-        <v>0.6848487144273757</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
+        <v>0.68484871442737572</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -3014,19 +3059,19 @@
         <v>12</v>
       </c>
       <c r="I8">
-        <v>-0.2597943666588219</v>
+        <v>-0.25979436665882188</v>
       </c>
       <c r="J8">
-        <v>0.3106354563374008</v>
+        <v>0.31063545633740081</v>
       </c>
       <c r="K8">
-        <v>-0.3056992027188027</v>
+        <v>-0.30569920271880269</v>
       </c>
       <c r="L8">
-        <v>0.3338931364506602</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+        <v>0.33389313645066021</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -3052,19 +3097,19 @@
         <v>100</v>
       </c>
       <c r="I9">
-        <v>-0.15625137459341</v>
+        <v>-0.15625137459340999</v>
       </c>
       <c r="J9">
-        <v>0.0301286154880051</v>
+        <v>3.0128615488005099E-2</v>
       </c>
       <c r="K9">
         <v>-0.2203331090972887</v>
       </c>
       <c r="L9">
-        <v>0.0276105659239954</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
+        <v>2.7610565923995401E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -3090,19 +3135,19 @@
         <v>50</v>
       </c>
       <c r="I10">
-        <v>-0.01391413642584883</v>
+        <v>-1.3914136425848831E-2</v>
       </c>
       <c r="J10">
-        <v>0.9090032366864784</v>
+        <v>0.90900323668647842</v>
       </c>
       <c r="K10">
-        <v>-0.01026612600739247</v>
+        <v>-1.0266126007392471E-2</v>
       </c>
       <c r="L10">
-        <v>0.9435901857829745</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
+        <v>0.94359018578297449</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -3128,19 +3173,19 @@
         <v>50</v>
       </c>
       <c r="I11">
-        <v>-0.02815294687312959</v>
+        <v>-2.8152946873129591E-2</v>
       </c>
       <c r="J11">
-        <v>0.8086800956106934</v>
+        <v>0.80868009561069343</v>
       </c>
       <c r="K11">
-        <v>-0.0299893827986723</v>
+        <v>-2.99893827986723E-2</v>
       </c>
       <c r="L11">
-        <v>0.8362130272367809</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
+        <v>0.83621302723678093</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -3166,19 +3211,19 @@
         <v>50</v>
       </c>
       <c r="I12">
-        <v>-0.247884667760308</v>
+        <v>-0.24788466776030799</v>
       </c>
       <c r="J12">
-        <v>0.03188792894690582</v>
+        <v>3.1887928946905821E-2</v>
       </c>
       <c r="K12">
-        <v>-0.3096184720415943</v>
+        <v>-0.30961847204159432</v>
       </c>
       <c r="L12">
-        <v>0.02866696147428332</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
+        <v>2.8666961474283319E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -3204,19 +3249,19 @@
         <v>10</v>
       </c>
       <c r="I13">
-        <v>-0.4787549991450212</v>
+        <v>-0.47875499914502118</v>
       </c>
       <c r="J13">
-        <v>0.07217560549492458</v>
+        <v>7.2175605494924577E-2</v>
       </c>
       <c r="K13">
-        <v>-0.6292853089020909</v>
+        <v>-0.62928530890209089</v>
       </c>
       <c r="L13">
-        <v>0.05124855216842294</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
+        <v>5.1248552168422938E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -3242,19 +3287,19 @@
         <v>10</v>
       </c>
       <c r="I14">
-        <v>-0.2267786838055363</v>
+        <v>-0.22677868380553631</v>
       </c>
       <c r="J14">
-        <v>0.3943870594034554</v>
+        <v>0.39438705940345542</v>
       </c>
       <c r="K14">
-        <v>-0.2860387767736777</v>
+        <v>-0.28603877677367773</v>
       </c>
       <c r="L14">
-        <v>0.4230203924441358</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
+        <v>0.42302039244413581</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -3283,16 +3328,16 @@
         <v>-0.1019294382875251</v>
       </c>
       <c r="J15">
-        <v>0.7040542681897126</v>
+        <v>0.70405426818971262</v>
       </c>
       <c r="K15">
-        <v>-0.0765092055676006</v>
+        <v>-7.6509205567600602E-2</v>
       </c>
       <c r="L15">
         <v>0.8336123677972922</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -3318,19 +3363,19 @@
         <v>10</v>
       </c>
       <c r="I16">
-        <v>-0.579545525280815</v>
+        <v>-0.57954552528081504</v>
       </c>
       <c r="J16">
-        <v>0.02951512807757192</v>
+        <v>2.9515128077571919E-2</v>
       </c>
       <c r="K16">
-        <v>-0.7119187333033755</v>
+        <v>-0.71191873330337552</v>
       </c>
       <c r="L16">
-        <v>0.02091481468718881</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
+        <v>2.091481468718881E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -3356,19 +3401,19 @@
         <v>10</v>
       </c>
       <c r="I17">
-        <v>-0.1259881576697424</v>
+        <v>-0.12598815766974239</v>
       </c>
       <c r="J17">
-        <v>0.6360988735986226</v>
+        <v>0.63609887359862261</v>
       </c>
       <c r="K17">
-        <v>-0.1906925178491184</v>
+        <v>-0.19069251784911839</v>
       </c>
       <c r="L17">
         <v>0.5977007516614028</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -3394,19 +3439,19 @@
         <v>10</v>
       </c>
       <c r="I18">
-        <v>0.579545525280815</v>
+        <v>0.57954552528081504</v>
       </c>
       <c r="J18">
-        <v>0.02951512807757192</v>
+        <v>2.9515128077571919E-2</v>
       </c>
       <c r="K18">
-        <v>0.7437008196115621</v>
+        <v>0.74370081961156209</v>
       </c>
       <c r="L18">
-        <v>0.01366958411527145</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
+        <v>1.3669584115271451E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -3432,19 +3477,19 @@
         <v>10</v>
       </c>
       <c r="I19">
-        <v>0.560611910581388</v>
+        <v>0.56061191058138804</v>
       </c>
       <c r="J19">
-        <v>0.0366903087793031</v>
+        <v>3.6690308779303099E-2</v>
       </c>
       <c r="K19">
-        <v>0.7172738021962557</v>
+        <v>0.71727380219625569</v>
       </c>
       <c r="L19">
-        <v>0.01954204435368506</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12">
+        <v>1.9542044353685058E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -3470,19 +3515,19 @@
         <v>10</v>
       </c>
       <c r="I20">
-        <v>-0.4787549991450212</v>
+        <v>-0.47875499914502118</v>
       </c>
       <c r="J20">
-        <v>0.07217560549492458</v>
+        <v>7.2175605494924577E-2</v>
       </c>
       <c r="K20">
-        <v>-0.6419981434253655</v>
+        <v>-0.64199814342536554</v>
       </c>
       <c r="L20">
-        <v>0.04536158917864154</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12">
+        <v>4.536158917864154E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -3508,19 +3553,19 @@
         <v>10</v>
       </c>
       <c r="I21">
-        <v>-0.2771739468734333</v>
+        <v>-0.27717394687343327</v>
       </c>
       <c r="J21">
-        <v>0.2978975979923409</v>
+        <v>0.29789759799234089</v>
       </c>
       <c r="K21">
-        <v>-0.3750286184365996</v>
+        <v>-0.37502861843659963</v>
       </c>
       <c r="L21">
-        <v>0.2855969029688312</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12">
+        <v>0.28559690296883122</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -3546,19 +3591,19 @@
         <v>10</v>
       </c>
       <c r="I22">
-        <v>0.1259881576697424</v>
+        <v>0.12598815766974239</v>
       </c>
       <c r="J22">
-        <v>0.6360988735986226</v>
+        <v>0.63609887359862261</v>
       </c>
       <c r="K22">
         <v>0.1461975970176575</v>
       </c>
       <c r="L22">
-        <v>0.6869410188538527</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12">
+        <v>0.68694101885385273</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -3584,19 +3629,19 @@
         <v>10</v>
       </c>
       <c r="I23">
-        <v>0.1259881576697424</v>
+        <v>0.12598815766974239</v>
       </c>
       <c r="J23">
-        <v>0.6360988735986226</v>
+        <v>0.63609887359862261</v>
       </c>
       <c r="K23">
-        <v>0.2161181868956676</v>
+        <v>0.21611818689566761</v>
       </c>
       <c r="L23">
-        <v>0.5487107060733141</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12">
+        <v>0.54871070607331407</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -3622,19 +3667,19 @@
         <v>10</v>
       </c>
       <c r="I24">
-        <v>-0.2267786838055363</v>
+        <v>-0.22677868380553631</v>
       </c>
       <c r="J24">
-        <v>0.3943870594034554</v>
+        <v>0.39438705940345542</v>
       </c>
       <c r="K24">
-        <v>-0.3114644458202268</v>
+        <v>-0.31146444582022681</v>
       </c>
       <c r="L24">
-        <v>0.3810089567050594</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12">
+        <v>0.38100895670505941</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -3660,19 +3705,19 @@
         <v>16</v>
       </c>
       <c r="I25">
-        <v>0.08475793795260131</v>
+        <v>8.4757937952601309E-2</v>
       </c>
       <c r="J25">
-        <v>0.6923284900281212</v>
+        <v>0.69232849002812125</v>
       </c>
       <c r="K25">
         <v>0.1099316484014564</v>
       </c>
       <c r="L25">
-        <v>0.685265005536689</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12">
+        <v>0.68526500553668901</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -3698,19 +3743,19 @@
         <v>16</v>
       </c>
       <c r="I26">
-        <v>0.08475793795260131</v>
+        <v>8.4757937952601309E-2</v>
       </c>
       <c r="J26">
-        <v>0.6923284900281212</v>
+        <v>0.69232849002812125</v>
       </c>
       <c r="K26">
         <v>0.1099316484014564</v>
       </c>
       <c r="L26">
-        <v>0.685265005536689</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12">
+        <v>0.68526500553668901</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -3736,19 +3781,19 @@
         <v>16</v>
       </c>
       <c r="I27">
-        <v>0.3404532748240978</v>
+        <v>0.34045327482409782</v>
       </c>
       <c r="J27">
         <v>0.1131965364706231</v>
       </c>
       <c r="K27">
-        <v>0.4029530171380015</v>
+        <v>0.40295301713800152</v>
       </c>
       <c r="L27">
         <v>0.1217337691688223</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -3774,19 +3819,19 @@
         <v>16</v>
       </c>
       <c r="I28">
-        <v>-0.4978586625371179</v>
+        <v>-0.49785866253711791</v>
       </c>
       <c r="J28">
-        <v>0.02133732054563453</v>
+        <v>2.1337320545634531E-2</v>
       </c>
       <c r="K28">
-        <v>-0.5769230769230769</v>
+        <v>-0.57692307692307687</v>
       </c>
       <c r="L28">
-        <v>0.01929785020805572</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12">
+        <v>1.929785020805572E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>18</v>
       </c>
@@ -3812,30 +3857,31 @@
         <v>16</v>
       </c>
       <c r="I29">
-        <v>-0.01695158759052026</v>
+        <v>-1.6951587590520258E-2</v>
       </c>
       <c r="J29">
-        <v>0.9369217280976989</v>
+        <v>0.93692172809769891</v>
       </c>
       <c r="K29">
-        <v>-0.03834824944236852</v>
+        <v>-3.8348249442368518E-2</v>
       </c>
       <c r="L29">
-        <v>0.8878693028318899</v>
+        <v>0.88786930283188992</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.7109375" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
@@ -3851,7 +3897,7 @@
     <col min="12" max="12" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3889,7 +3935,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -3915,7 +3961,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -3941,7 +3987,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -3967,7 +4013,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -3993,7 +4039,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -4019,7 +4065,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -4045,7 +4091,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -4071,7 +4117,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -4100,16 +4146,16 @@
         <v>-0.1325530043077417</v>
       </c>
       <c r="J9">
-        <v>0.1086826442074059</v>
+        <v>0.10868264420740591</v>
       </c>
       <c r="K9">
-        <v>-0.1612223880273475</v>
+        <v>-0.16122238802734751</v>
       </c>
       <c r="L9">
         <v>0.1090548020620709</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -4135,19 +4181,19 @@
         <v>50</v>
       </c>
       <c r="I10">
-        <v>-0.004001088444105332</v>
+        <v>-4.0010884441053322E-3</v>
       </c>
       <c r="J10">
-        <v>0.9739374982488735</v>
+        <v>0.97393749824887355</v>
       </c>
       <c r="K10">
-        <v>-0.004014544573191041</v>
+        <v>-4.0145445731910407E-3</v>
       </c>
       <c r="L10">
-        <v>0.9779259755977681</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
+        <v>0.97792597559776806</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -4173,19 +4219,19 @@
         <v>50</v>
       </c>
       <c r="I11">
-        <v>-0.01888959038201153</v>
+        <v>-1.8889590382011531E-2</v>
       </c>
       <c r="J11">
         <v>0.8717029852220165</v>
       </c>
       <c r="K11">
-        <v>-0.02206154843492711</v>
+        <v>-2.2061548434927108E-2</v>
       </c>
       <c r="L11">
-        <v>0.8791305588586364</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
+        <v>0.87913055885863645</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -4211,19 +4257,19 @@
         <v>50</v>
       </c>
       <c r="I12">
-        <v>-0.2476064162497625</v>
+        <v>-0.24760641624976251</v>
       </c>
       <c r="J12">
-        <v>0.0331142128596994</v>
+        <v>3.3114212859699399E-2</v>
       </c>
       <c r="K12">
-        <v>-0.3099127537051835</v>
+        <v>-0.30991275370518351</v>
       </c>
       <c r="L12">
-        <v>0.02850794708171081</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
+        <v>2.850794708171081E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -4261,7 +4307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -4290,16 +4336,16 @@
         <v>0.6085806194501846</v>
       </c>
       <c r="J14">
-        <v>0.03300625766123251</v>
+        <v>3.300625766123251E-2</v>
       </c>
       <c r="K14">
-        <v>0.7106690545187014</v>
+        <v>0.71066905451870144</v>
       </c>
       <c r="L14">
-        <v>0.02124449212877441</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
+        <v>2.1244492128774412E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -4325,19 +4371,19 @@
         <v>10</v>
       </c>
       <c r="I15">
-        <v>0.6770032003863301</v>
+        <v>0.67700320038633011</v>
       </c>
       <c r="J15">
-        <v>0.01865536081150319</v>
+        <v>1.865536081150319E-2</v>
       </c>
       <c r="K15">
-        <v>0.7841156792042765</v>
+        <v>0.78411567920427649</v>
       </c>
       <c r="L15">
-        <v>0.007255789526699558</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
+        <v>7.2557895266995576E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -4366,16 +4412,16 @@
         <v>-0.1217161238900369</v>
       </c>
       <c r="J16">
-        <v>0.6698153575994166</v>
+        <v>0.66981535759941657</v>
       </c>
       <c r="K16">
         <v>-0.1421338109037403</v>
       </c>
       <c r="L16">
-        <v>0.6952876854012655</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
+        <v>0.69528768540126551</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -4404,16 +4450,16 @@
         <v>-0.3042903097250923</v>
       </c>
       <c r="J17">
-        <v>0.2864220227778588</v>
+        <v>0.28642202277785878</v>
       </c>
       <c r="K17">
-        <v>-0.3553345272593507</v>
+        <v>-0.35533452725935072</v>
       </c>
       <c r="L17">
-        <v>0.3136373640754537</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
+        <v>0.31363736407545367</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -4439,19 +4485,19 @@
         <v>10</v>
       </c>
       <c r="I18">
-        <v>0.06085806194501846</v>
+        <v>6.0858061945018457E-2</v>
       </c>
       <c r="J18">
-        <v>0.8311704095417624</v>
+        <v>0.83117040954176236</v>
       </c>
       <c r="K18">
-        <v>0.07106690545187015</v>
+        <v>7.1066905451870152E-2</v>
       </c>
       <c r="L18">
-        <v>0.8453239136912953</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
+        <v>0.84532391369129534</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -4477,19 +4523,19 @@
         <v>10</v>
       </c>
       <c r="I19">
-        <v>0.09231861823449956</v>
+        <v>9.2318618234499564E-2</v>
       </c>
       <c r="J19">
-        <v>0.7483812122920345</v>
+        <v>0.74838121229203447</v>
       </c>
       <c r="K19">
-        <v>0.1069248653460377</v>
+        <v>0.10692486534603771</v>
       </c>
       <c r="L19">
-        <v>0.7687577033932652</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12">
+        <v>0.76875770339326521</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -4515,19 +4561,19 @@
         <v>10</v>
       </c>
       <c r="I20">
-        <v>-0.06085806194501846</v>
+        <v>-6.0858061945018457E-2</v>
       </c>
       <c r="J20">
-        <v>0.8311704095417624</v>
+        <v>0.83117040954176236</v>
       </c>
       <c r="K20">
-        <v>-0.07106690545187015</v>
+        <v>-7.1066905451870152E-2</v>
       </c>
       <c r="L20">
-        <v>0.8453239136912953</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12">
+        <v>0.84532391369129534</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -4553,19 +4599,19 @@
         <v>10</v>
       </c>
       <c r="I21">
-        <v>-0.2434322477800739</v>
+        <v>-0.24343224778007391</v>
       </c>
       <c r="J21">
-        <v>0.3937686346429927</v>
+        <v>0.39376863464299272</v>
       </c>
       <c r="K21">
-        <v>-0.2842676218074806</v>
+        <v>-0.28426762180748061</v>
       </c>
       <c r="L21">
-        <v>0.4260244484285426</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12">
+        <v>0.42602444842854259</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -4594,16 +4640,16 @@
         <v>0.1217161238900369</v>
       </c>
       <c r="J22">
-        <v>0.6698153575994166</v>
+        <v>0.66981535759941657</v>
       </c>
       <c r="K22">
         <v>0.1421338109037403</v>
       </c>
       <c r="L22">
-        <v>0.6952876854012655</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12">
+        <v>0.69528768540126551</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -4629,19 +4675,19 @@
         <v>10</v>
       </c>
       <c r="I23">
-        <v>0.2434322477800739</v>
+        <v>0.24343224778007391</v>
       </c>
       <c r="J23">
-        <v>0.3937686346429927</v>
+        <v>0.39376863464299272</v>
       </c>
       <c r="K23">
-        <v>0.2842676218074806</v>
+        <v>0.28426762180748061</v>
       </c>
       <c r="L23">
-        <v>0.4260244484285426</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12">
+        <v>0.42602444842854259</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -4667,19 +4713,19 @@
         <v>10</v>
       </c>
       <c r="I24">
-        <v>-0.2434322477800739</v>
+        <v>-0.24343224778007391</v>
       </c>
       <c r="J24">
-        <v>0.3937686346429927</v>
+        <v>0.39376863464299272</v>
       </c>
       <c r="K24">
-        <v>-0.2842676218074806</v>
+        <v>-0.28426762180748061</v>
       </c>
       <c r="L24">
-        <v>0.4260244484285426</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12">
+        <v>0.42602444842854259</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -4705,19 +4751,19 @@
         <v>16</v>
       </c>
       <c r="I25">
-        <v>-0.3535533905932737</v>
+        <v>-0.35355339059327368</v>
       </c>
       <c r="J25">
         <v>0.1037416782365415</v>
       </c>
       <c r="K25">
-        <v>-0.4200840252084029</v>
+        <v>-0.42008402520840288</v>
       </c>
       <c r="L25">
         <v>0.105228057983522</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -4743,19 +4789,19 @@
         <v>16</v>
       </c>
       <c r="I26">
-        <v>-0.1649915822768611</v>
+        <v>-0.16499158227686109</v>
       </c>
       <c r="J26">
         <v>0.4476990724652935</v>
       </c>
       <c r="K26">
-        <v>-0.1960392117639214</v>
+        <v>-0.19603921176392139</v>
       </c>
       <c r="L26">
         <v>0.4668248490265503</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -4781,19 +4827,19 @@
         <v>16</v>
       </c>
       <c r="I27">
-        <v>0.02366905341655754</v>
+        <v>2.3669053416557541E-2</v>
       </c>
       <c r="J27">
-        <v>0.9135633303377861</v>
+        <v>0.91356333033778614</v>
       </c>
       <c r="K27">
-        <v>0.02802621677476181</v>
+        <v>2.802621677476181E-2</v>
       </c>
       <c r="L27">
-        <v>0.9179387985999929</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12">
+        <v>0.91793879859999294</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -4819,19 +4865,19 @@
         <v>16</v>
       </c>
       <c r="I28">
-        <v>-0.2625754538144587</v>
+        <v>-0.26257545381445868</v>
       </c>
       <c r="J28">
-        <v>0.2314460271038938</v>
+        <v>0.23144602710389381</v>
       </c>
       <c r="K28">
-        <v>-0.3089716991054783</v>
+        <v>-0.30897169910547828</v>
       </c>
       <c r="L28">
-        <v>0.2442606266224961</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12">
+        <v>0.24426062662249609</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>18</v>
       </c>
@@ -4857,13 +4903,13 @@
         <v>16</v>
       </c>
       <c r="I29">
-        <v>0.2592724864350675</v>
+        <v>0.25927248643506751</v>
       </c>
       <c r="J29">
         <v>0.2328233516916538</v>
       </c>
       <c r="K29">
-        <v>0.3080616184861621</v>
+        <v>0.30806161848616209</v>
       </c>
       <c r="L29">
         <v>0.2457251662216493</v>
@@ -4871,16 +4917,17 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.7109375" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
@@ -4896,7 +4943,7 @@
     <col min="12" max="12" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4934,7 +4981,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -4960,7 +5007,7 @@
         <v>23</v>
       </c>
       <c r="I2">
-        <v>-0.2588600915717736</v>
+        <v>-0.25886009157177359</v>
       </c>
       <c r="J2">
         <v>0.1185826134820492</v>
@@ -4972,7 +5019,7 @@
         <v>0.157096814687567</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -5001,16 +5048,16 @@
         <v>-0.3630554894720564</v>
       </c>
       <c r="J3">
-        <v>0.02649782086730554</v>
+        <v>2.6497820867305542E-2</v>
       </c>
       <c r="K3">
-        <v>-0.4471228632493155</v>
+        <v>-0.44712286324931549</v>
       </c>
       <c r="L3">
-        <v>0.03242678547292783</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+        <v>3.2426785472927828E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -5036,19 +5083,19 @@
         <v>23</v>
       </c>
       <c r="I4">
-        <v>0.3826849293392768</v>
+        <v>0.38268492933927678</v>
       </c>
       <c r="J4">
-        <v>0.01856470797931634</v>
+        <v>1.856470797931634E-2</v>
       </c>
       <c r="K4">
-        <v>0.4532739558663172</v>
+        <v>0.45327395586631719</v>
       </c>
       <c r="L4">
-        <v>0.0298421137496698</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
+        <v>2.9842113749669798E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -5077,16 +5124,16 @@
         <v>-0.2018433569398328</v>
       </c>
       <c r="J5">
-        <v>0.4065712940338708</v>
+        <v>0.40657129403387082</v>
       </c>
       <c r="K5">
         <v>-0.2056848110006326</v>
       </c>
       <c r="L5">
-        <v>0.521309719682044</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
+        <v>0.52130971968204398</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -5112,10 +5159,10 @@
         <v>12</v>
       </c>
       <c r="I6">
-        <v>-0.2385421491107114</v>
+        <v>-0.23854214911071139</v>
       </c>
       <c r="J6">
-        <v>0.326671088638757</v>
+        <v>0.32667108863875699</v>
       </c>
       <c r="K6">
         <v>-0.2437745908155646</v>
@@ -5124,7 +5171,7 @@
         <v>0.4451488240391529</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -5150,19 +5197,19 @@
         <v>12</v>
       </c>
       <c r="I7">
-        <v>-0.4954336943068622</v>
+        <v>-0.49543369430686218</v>
       </c>
       <c r="J7">
-        <v>0.0416368567827736</v>
+        <v>4.1636856782773603E-2</v>
       </c>
       <c r="K7">
-        <v>-0.5561107852980067</v>
+        <v>-0.55611078529800673</v>
       </c>
       <c r="L7">
-        <v>0.06043495620092659</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
+        <v>6.0434956200926593E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -5188,19 +5235,19 @@
         <v>12</v>
       </c>
       <c r="I8">
-        <v>0.3486385256233475</v>
+        <v>0.34863852562334752</v>
       </c>
       <c r="J8">
-        <v>0.1517044197305971</v>
+        <v>0.15170441973059709</v>
       </c>
       <c r="K8">
-        <v>0.4037516660382788</v>
+        <v>0.40375166603827878</v>
       </c>
       <c r="L8">
-        <v>0.1930534976448194</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+        <v>0.19305349764481941</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -5229,16 +5276,16 @@
         <v>-0.1508932577851104</v>
       </c>
       <c r="J9">
-        <v>0.03976539977998658</v>
+        <v>3.9765399779986582E-2</v>
       </c>
       <c r="K9">
-        <v>-0.2101007063448729</v>
+        <v>-0.21010070634487291</v>
       </c>
       <c r="L9">
-        <v>0.03589890255176344</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
+        <v>3.5898902551763437E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -5264,19 +5311,19 @@
         <v>50</v>
       </c>
       <c r="I10">
-        <v>-0.02584053907657639</v>
+        <v>-2.584053907657639E-2</v>
       </c>
       <c r="J10">
-        <v>0.8319012317886401</v>
+        <v>0.83190123178864006</v>
       </c>
       <c r="K10">
-        <v>-0.02491868767248899</v>
+        <v>-2.491868767248899E-2</v>
       </c>
       <c r="L10">
-        <v>0.8636170341288709</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
+        <v>0.86361703412887092</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -5302,19 +5349,19 @@
         <v>50</v>
       </c>
       <c r="I11">
-        <v>-0.02439922062337898</v>
+        <v>-2.439922062337898E-2</v>
       </c>
       <c r="J11">
-        <v>0.8337884478927275</v>
+        <v>0.83378844789272755</v>
       </c>
       <c r="K11">
-        <v>-0.02888208251072132</v>
+        <v>-2.8882082510721319E-2</v>
       </c>
       <c r="L11">
-        <v>0.8421820698041393</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
+        <v>0.84218206980413934</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -5340,19 +5387,19 @@
         <v>50</v>
       </c>
       <c r="I12">
-        <v>-0.2516122567491849</v>
+        <v>-0.25161225674918491</v>
       </c>
       <c r="J12">
-        <v>0.02940004335865699</v>
+        <v>2.940004335865699E-2</v>
       </c>
       <c r="K12">
-        <v>-0.311094163299463</v>
+        <v>-0.31109416329946299</v>
       </c>
       <c r="L12">
-        <v>0.02787696039183273</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
+        <v>2.7876960391832729E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -5378,19 +5425,19 @@
         <v>10</v>
       </c>
       <c r="I13">
-        <v>0.04969039949999533</v>
+        <v>4.9690399499995333E-2</v>
       </c>
       <c r="J13">
-        <v>0.8509806870320558</v>
+        <v>0.85098068703205576</v>
       </c>
       <c r="K13">
-        <v>0.01262892050706804</v>
+        <v>1.262892050706804E-2</v>
       </c>
       <c r="L13">
-        <v>0.9723786419920799</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
+        <v>0.97237864199207991</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -5416,19 +5463,19 @@
         <v>10</v>
       </c>
       <c r="I14">
-        <v>-0.149071198499986</v>
+        <v>-0.14907119849998601</v>
       </c>
       <c r="J14">
-        <v>0.5730251193553904</v>
+        <v>0.57302511935539036</v>
       </c>
       <c r="K14">
         <v>-0.1894338076060206</v>
       </c>
       <c r="L14">
-        <v>0.6001664342511973</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
+        <v>0.60016643425119731</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -5454,19 +5501,19 @@
         <v>10</v>
       </c>
       <c r="I15">
-        <v>-0.1256297269074015</v>
+        <v>-0.12562972690740151</v>
       </c>
       <c r="J15">
-        <v>0.6374017405958849</v>
+        <v>0.63740174059588495</v>
       </c>
       <c r="K15">
-        <v>-0.152008377581442</v>
+        <v>-0.15200837758144201</v>
       </c>
       <c r="L15">
-        <v>0.6750590889374006</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
+        <v>0.67505908893740063</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -5492,19 +5539,19 @@
         <v>10</v>
       </c>
       <c r="I16">
-        <v>-0.298142396999972</v>
+        <v>-0.29814239699997203</v>
       </c>
       <c r="J16">
-        <v>0.2596563563704499</v>
+        <v>0.25965635637044993</v>
       </c>
       <c r="K16">
-        <v>-0.3788676152120412</v>
+        <v>-0.37886761521204121</v>
       </c>
       <c r="L16">
-        <v>0.2802942824523375</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
+        <v>0.28029428245233751</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -5533,16 +5580,16 @@
         <v>-0.1987615979999813</v>
       </c>
       <c r="J17">
-        <v>0.4523703606773608</v>
+        <v>0.45237036067736081</v>
       </c>
       <c r="K17">
-        <v>-0.3409808536908371</v>
+        <v>-0.34098085369083708</v>
       </c>
       <c r="L17">
-        <v>0.3349456951179903</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
+        <v>0.33494569511799033</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -5568,19 +5615,19 @@
         <v>10</v>
       </c>
       <c r="I18">
-        <v>0.149071198499986</v>
+        <v>0.14907119849998601</v>
       </c>
       <c r="J18">
-        <v>0.5730251193553904</v>
+        <v>0.57302511935539036</v>
       </c>
       <c r="K18">
-        <v>0.1641759665918845</v>
+        <v>0.16417596659188449</v>
       </c>
       <c r="L18">
-        <v>0.6503895621649565</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
+        <v>0.65038956216495647</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -5606,19 +5653,19 @@
         <v>10</v>
       </c>
       <c r="I19">
-        <v>0.07537783614444091</v>
+        <v>7.5377836144440907E-2</v>
       </c>
       <c r="J19">
-        <v>0.7773295263554205</v>
+        <v>0.77732952635542052</v>
       </c>
       <c r="K19">
         <v>0.1076726007868547</v>
       </c>
       <c r="L19">
-        <v>0.7671778789420547</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12">
+        <v>0.76717787894205469</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -5644,19 +5691,19 @@
         <v>10</v>
       </c>
       <c r="I20">
-        <v>-0.09938079899999065</v>
+        <v>-9.9380798999990652E-2</v>
       </c>
       <c r="J20">
         <v>0.7071142312899612</v>
       </c>
       <c r="K20">
-        <v>-0.1262892050706804</v>
+        <v>-0.12628920507068039</v>
       </c>
       <c r="L20">
-        <v>0.7281063840216824</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12">
+        <v>0.72810638402168237</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -5682,19 +5729,19 @@
         <v>10</v>
       </c>
       <c r="I21">
-        <v>-0.149071198499986</v>
+        <v>-0.14907119849998601</v>
       </c>
       <c r="J21">
-        <v>0.5730251193553904</v>
+        <v>0.57302511935539036</v>
       </c>
       <c r="K21">
         <v>-0.2399494896342928</v>
       </c>
       <c r="L21">
-        <v>0.5043017190353258</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12">
+        <v>0.50430171903532583</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -5720,19 +5767,19 @@
         <v>10</v>
       </c>
       <c r="I22">
-        <v>0.3975231959999626</v>
+        <v>0.39752319599996261</v>
       </c>
       <c r="J22">
         <v>0.1328549557310538</v>
       </c>
       <c r="K22">
-        <v>0.5304146612968577</v>
+        <v>0.53041466129685766</v>
       </c>
       <c r="L22">
         <v>0.1147392659290222</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -5758,19 +5805,19 @@
         <v>10</v>
       </c>
       <c r="I23">
-        <v>0.298142396999972</v>
+        <v>0.29814239699997203</v>
       </c>
       <c r="J23">
-        <v>0.2596563563704499</v>
+        <v>0.25965635637044993</v>
       </c>
       <c r="K23">
-        <v>0.4041254562261773</v>
+        <v>0.40412545622617729</v>
       </c>
       <c r="L23">
-        <v>0.2467547295422347</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12">
+        <v>0.24675472954223471</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -5799,16 +5846,16 @@
         <v>-0.2484519974999766</v>
       </c>
       <c r="J24">
-        <v>0.347558036741169</v>
+        <v>0.34755803674116897</v>
       </c>
       <c r="K24">
-        <v>-0.4293832972403134</v>
+        <v>-0.42938329724031338</v>
       </c>
       <c r="L24">
-        <v>0.2155824117700313</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12">
+        <v>0.21558241177003129</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -5834,7 +5881,7 @@
         <v>16</v>
       </c>
       <c r="I25">
-        <v>-0.31352722326441</v>
+        <v>-0.31352722326441002</v>
       </c>
       <c r="J25">
         <v>0.1131685336545776</v>
@@ -5843,10 +5890,10 @@
         <v>-0.4479914656638877</v>
       </c>
       <c r="L25">
-        <v>0.08182143505121871</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12">
+        <v>8.1821435051218708E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -5875,16 +5922,16 @@
         <v>-0.3872983346207417</v>
       </c>
       <c r="J26">
-        <v>0.05036597579032801</v>
+        <v>5.0365975790328012E-2</v>
       </c>
       <c r="K26">
-        <v>-0.5070173682344674</v>
+        <v>-0.50701736823446741</v>
       </c>
       <c r="L26">
-        <v>0.04501930875693567</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12">
+        <v>4.5019308756935668E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -5910,19 +5957,19 @@
         <v>16</v>
       </c>
       <c r="I27">
-        <v>0.08334047874242113</v>
+        <v>8.3340478742421134E-2</v>
       </c>
       <c r="J27">
         <v>0.6747078413451294</v>
       </c>
       <c r="K27">
-        <v>0.08027373462987823</v>
+        <v>8.0273734629878232E-2</v>
       </c>
       <c r="L27">
-        <v>0.7675926515511813</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12">
+        <v>0.76759265155118128</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -5948,19 +5995,19 @@
         <v>16</v>
       </c>
       <c r="I28">
-        <v>0.09338863578008762</v>
+        <v>9.3388635780087617E-2</v>
       </c>
       <c r="J28">
-        <v>0.6401498414586226</v>
+        <v>0.64014984145862264</v>
       </c>
       <c r="K28">
         <v>0.1305442024324843</v>
       </c>
       <c r="L28">
-        <v>0.6298840619248964</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12">
+        <v>0.62988406192489643</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>18</v>
       </c>
@@ -5986,19 +6033,20 @@
         <v>16</v>
       </c>
       <c r="I29">
-        <v>0.1290994448735805</v>
+        <v>0.12909944487358049</v>
       </c>
       <c r="J29">
-        <v>0.5142199988155506</v>
+        <v>0.51421999881555058</v>
       </c>
       <c r="K29">
-        <v>0.1619428608987702</v>
+        <v>0.16194286089877019</v>
       </c>
       <c r="L29">
-        <v>0.5490376092324329</v>
+        <v>0.54903760923243294</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>